<commit_message>
working through most recent pH data. Precision looks great. Accuracy looks ok. Would be nice to be better on that but will have to accept for now.
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/20201103 pH check sample results summary.xlsx
+++ b/check sample work/pH QAQC/20201103 pH check sample results summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="example to follow" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="305">
   <si>
     <t>sample</t>
   </si>
@@ -885,6 +885,66 @@
   </si>
   <si>
     <t xml:space="preserve"> BAYSTD1-11032020-2-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> baystd1-epp-11092020-1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> baystd1-epp-11092020-2-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> baystd1-stck-11092020-3-G</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> baystd1-stck-11092020-4-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B-0043-C1-P3-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B-0043-C1-P4-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0028-C2-P3-G</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0028-C2-P4-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M-0049-C1-P3-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M-0049-C1-P4-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0044-C1-P3-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0044-C1-P4-E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DIC-11-10-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0078-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0078-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0078-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0078-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0078-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0078-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0078-7</t>
   </si>
 </sst>
 </file>
@@ -2094,11 +2154,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O228"/>
+  <dimension ref="A1:O248"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G226" sqref="G226:N226"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E241" activeCellId="2" sqref="A241 D241 E241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7759,6 +7819,510 @@
         <v>275</v>
       </c>
     </row>
+    <row r="229" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="B229" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D229" s="15">
+        <v>7.9630303411878298</v>
+      </c>
+      <c r="E229" s="15">
+        <v>7.7713262449962803</v>
+      </c>
+      <c r="G229" s="15">
+        <f>AVERAGE(D229:D230)</f>
+        <v>7.9169510651725901</v>
+      </c>
+      <c r="H229" s="14">
+        <f>_xlfn.STDEV.S(D229:D230)</f>
+        <v>6.5165937085085335E-2</v>
+      </c>
+      <c r="I229" s="14">
+        <f>2*H229</f>
+        <v>0.13033187417017067</v>
+      </c>
+      <c r="J229" s="14">
+        <f>H229/G229</f>
+        <v>8.2311910922067463E-3</v>
+      </c>
+      <c r="K229" s="19">
+        <f>J229</f>
+        <v>8.2311910922067463E-3</v>
+      </c>
+      <c r="L229" s="15">
+        <f>MIN(D229:D230)</f>
+        <v>7.8708717891573503</v>
+      </c>
+      <c r="M229" s="15">
+        <f>MAX(D229:D230)</f>
+        <v>7.9630303411878298</v>
+      </c>
+      <c r="N229" s="14">
+        <f>M229-L229</f>
+        <v>9.2158552030479512E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B230" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D230" s="15">
+        <v>7.8708717891573503</v>
+      </c>
+      <c r="E230" s="15">
+        <v>7.6791676929657999</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B231" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D231" s="15">
+        <v>7.8791164786535397</v>
+      </c>
+      <c r="E231" s="15">
+        <v>7.6874123824619902</v>
+      </c>
+      <c r="G231" s="15">
+        <f>AVERAGE(D231:D232)</f>
+        <v>7.8708697321498295</v>
+      </c>
+      <c r="H231" s="14">
+        <f>_xlfn.STDEV.S(D231:D232)</f>
+        <v>1.1662660750999178E-2</v>
+      </c>
+      <c r="I231" s="14">
+        <f>2*H231</f>
+        <v>2.3325321501998356E-2</v>
+      </c>
+      <c r="J231" s="14">
+        <f>H231/G231</f>
+        <v>1.4817499396999508E-3</v>
+      </c>
+      <c r="K231" s="19">
+        <f>J231</f>
+        <v>1.4817499396999508E-3</v>
+      </c>
+      <c r="L231" s="15">
+        <f>MIN(D231:D232)</f>
+        <v>7.8626229856461203</v>
+      </c>
+      <c r="M231" s="15">
+        <f>MAX(D231:D232)</f>
+        <v>7.8791164786535397</v>
+      </c>
+      <c r="N231" s="14">
+        <f>M231-L231</f>
+        <v>1.6493493007419424E-2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="B232" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D232" s="15">
+        <v>7.8626229856461203</v>
+      </c>
+      <c r="E232" s="15">
+        <v>7.6709188894545699</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="B233" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D233" s="15">
+        <v>7.9715277814184304</v>
+      </c>
+      <c r="E233" s="15">
+        <v>7.8573703834465096</v>
+      </c>
+      <c r="G233" s="15">
+        <f>AVERAGE(D233:D234)</f>
+        <v>7.9727850025090801</v>
+      </c>
+      <c r="H233" s="14">
+        <f>_xlfn.STDEV.S(D233:D234)</f>
+        <v>1.7779791172982003E-3</v>
+      </c>
+      <c r="I233" s="14">
+        <f>2*H233</f>
+        <v>3.5559582345964006E-3</v>
+      </c>
+      <c r="J233" s="14">
+        <f>H233/G233</f>
+        <v>2.230060282245991E-4</v>
+      </c>
+      <c r="K233" s="19">
+        <f>J233</f>
+        <v>2.230060282245991E-4</v>
+      </c>
+      <c r="L233" s="15">
+        <f>MIN(D233:D234)</f>
+        <v>7.9715277814184304</v>
+      </c>
+      <c r="M233" s="15">
+        <f>MAX(D233:D234)</f>
+        <v>7.9740422235997297</v>
+      </c>
+      <c r="N233" s="14">
+        <f>M233-L233</f>
+        <v>2.514442181299259E-3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B234" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D234" s="15">
+        <v>7.9740422235997297</v>
+      </c>
+      <c r="E234" s="15">
+        <v>7.8598848256278</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B235" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D235" s="15">
+        <v>7.9776760457288001</v>
+      </c>
+      <c r="E235" s="15">
+        <v>7.8351774522553201</v>
+      </c>
+      <c r="G235" s="15">
+        <f>AVERAGE(D235:D236)</f>
+        <v>7.9790685368239753</v>
+      </c>
+      <c r="H235" s="14">
+        <f>_xlfn.STDEV.S(D235:D236)</f>
+        <v>1.9692797922799782E-3</v>
+      </c>
+      <c r="I235" s="14">
+        <f>2*H235</f>
+        <v>3.9385595845599563E-3</v>
+      </c>
+      <c r="J235" s="14">
+        <f>H235/G235</f>
+        <v>2.468057246521458E-4</v>
+      </c>
+      <c r="K235" s="19">
+        <f>J235</f>
+        <v>2.468057246521458E-4</v>
+      </c>
+      <c r="L235" s="15">
+        <f>MIN(D235:D236)</f>
+        <v>7.9776760457288001</v>
+      </c>
+      <c r="M235" s="15">
+        <f>MAX(D235:D236)</f>
+        <v>7.9804610279191497</v>
+      </c>
+      <c r="N235" s="14">
+        <f>M235-L235</f>
+        <v>2.7849821903496164E-3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="B236" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D236" s="15">
+        <v>7.9804610279191497</v>
+      </c>
+      <c r="E236" s="15">
+        <v>7.8379624344456804</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B237" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D237" s="15">
+        <v>7.97955183325492</v>
+      </c>
+      <c r="E237" s="15">
+        <v>7.8765329502265304</v>
+      </c>
+      <c r="G237" s="15">
+        <f>AVERAGE(D237:D238)</f>
+        <v>7.9767527392051898</v>
+      </c>
+      <c r="H237" s="14">
+        <f>_xlfn.STDEV.S(D237:D238)</f>
+        <v>3.9585167674863102E-3</v>
+      </c>
+      <c r="I237" s="14">
+        <f>2*H237</f>
+        <v>7.9170335349726204E-3</v>
+      </c>
+      <c r="J237" s="14">
+        <f>H237/G237</f>
+        <v>4.9625667197009549E-4</v>
+      </c>
+      <c r="K237" s="19">
+        <f>J237</f>
+        <v>4.9625667197009549E-4</v>
+      </c>
+      <c r="L237" s="15">
+        <f>MIN(D237:D238)</f>
+        <v>7.9739536451554596</v>
+      </c>
+      <c r="M237" s="15">
+        <f>MAX(D237:D238)</f>
+        <v>7.97955183325492</v>
+      </c>
+      <c r="N237" s="14">
+        <f>M237-L237</f>
+        <v>5.5981880994604438E-3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B238" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D238" s="15">
+        <v>7.9739536451554596</v>
+      </c>
+      <c r="E238" s="15">
+        <v>7.87093476212707</v>
+      </c>
+    </row>
+    <row r="239" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B239" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D239" s="15">
+        <v>7.97377413348151</v>
+      </c>
+      <c r="E239" s="15">
+        <v>7.8832849921922197</v>
+      </c>
+      <c r="G239" s="15">
+        <f>AVERAGE(D239:D240)</f>
+        <v>7.9740437379359701</v>
+      </c>
+      <c r="H239" s="14">
+        <f>_xlfn.STDEV.S(D239:D240)</f>
+        <v>3.8127827597369418E-4</v>
+      </c>
+      <c r="I239" s="14">
+        <f>2*H239</f>
+        <v>7.6255655194738836E-4</v>
+      </c>
+      <c r="J239" s="14">
+        <f>H239/G239</f>
+        <v>4.7814921576086765E-5</v>
+      </c>
+      <c r="K239" s="19">
+        <f>J239</f>
+        <v>4.7814921576086765E-5</v>
+      </c>
+      <c r="L239" s="15">
+        <f>MIN(D239:D240)</f>
+        <v>7.97377413348151</v>
+      </c>
+      <c r="M239" s="15">
+        <f>MAX(D239:D240)</f>
+        <v>7.9743133423904302</v>
+      </c>
+      <c r="N239" s="14">
+        <f>M239-L239</f>
+        <v>5.392089089202301E-4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="B240" s="18">
+        <v>44144</v>
+      </c>
+      <c r="D240" s="15">
+        <v>7.9743133423904302</v>
+      </c>
+      <c r="E240" s="15">
+        <v>7.8838242011011399</v>
+      </c>
+    </row>
+    <row r="241" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="B241" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D241" s="15">
+        <v>8.1335197047369494</v>
+      </c>
+      <c r="E241" s="15">
+        <v>8.1335197047369494</v>
+      </c>
+    </row>
+    <row r="242" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B242" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D242" s="15">
+        <v>7.87820718412478</v>
+      </c>
+      <c r="E242" s="15">
+        <v>7.7181559493774703</v>
+      </c>
+      <c r="G242" s="15">
+        <f>AVERAGE(D242:D248)</f>
+        <v>7.8773527118531925</v>
+      </c>
+      <c r="H242" s="14">
+        <f>_xlfn.STDEV.S(D242:D248)</f>
+        <v>1.1293541813510387E-3</v>
+      </c>
+      <c r="I242" s="14">
+        <f>2*H242</f>
+        <v>2.2587083627020775E-3</v>
+      </c>
+      <c r="J242" s="14">
+        <f>H242/G242</f>
+        <v>1.4336722280464597E-4</v>
+      </c>
+      <c r="K242" s="19">
+        <f>J242</f>
+        <v>1.4336722280464597E-4</v>
+      </c>
+      <c r="L242" s="15">
+        <f>MIN(D242:D243)</f>
+        <v>7.8751451622983097</v>
+      </c>
+      <c r="M242" s="15">
+        <f>MAX(D242:D243)</f>
+        <v>7.87820718412478</v>
+      </c>
+      <c r="N242" s="14">
+        <f>M242-L242</f>
+        <v>3.062021826470307E-3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B243" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D243" s="15">
+        <v>7.8751451622983097</v>
+      </c>
+      <c r="E243" s="15">
+        <v>7.715093927551</v>
+      </c>
+    </row>
+    <row r="244" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B244" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D244" s="15">
+        <v>7.8782839673411598</v>
+      </c>
+      <c r="E244" s="15">
+        <v>7.71823273259385</v>
+      </c>
+    </row>
+    <row r="245" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="B245" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D245" s="15">
+        <v>7.8765364051709197</v>
+      </c>
+      <c r="E245" s="15">
+        <v>7.7164851704236099</v>
+      </c>
+    </row>
+    <row r="246" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="B246" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D246" s="15">
+        <v>7.8777392762071701</v>
+      </c>
+      <c r="E246" s="15">
+        <v>7.7176880414598603</v>
+      </c>
+    </row>
+    <row r="247" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B247" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D247" s="15">
+        <v>7.8777358254843204</v>
+      </c>
+      <c r="E247" s="15">
+        <v>7.7176845907370097</v>
+      </c>
+    </row>
+    <row r="248" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B248" s="18">
+        <v>44145</v>
+      </c>
+      <c r="D248" s="15">
+        <v>7.8778211623456897</v>
+      </c>
+      <c r="E248" s="15">
+        <v>7.7177699275983898</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O191"/>
   <sortState ref="A2:O144">
@@ -7773,9 +8337,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7875,11 +8439,11 @@
         <v>8.1049089149999993</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C10" si="0">$L$2</f>
+        <f t="shared" ref="C3:C11" si="0">$L$2</f>
         <v>8.0935490943465993</v>
       </c>
       <c r="D3" s="12">
-        <f t="shared" ref="D3:D10" si="1">B3-C3</f>
+        <f t="shared" ref="D3:D11" si="1">B3-C3</f>
         <v>1.1359820653400021E-2</v>
       </c>
       <c r="E3" s="13">
@@ -7888,7 +8452,7 @@
       </c>
       <c r="G3">
         <f>SQRT(SUM(E2:E46)/ROWS(E2:E46))</f>
-        <v>8.7728419526337444E-3</v>
+        <v>1.0605002710086344E-2</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -7945,7 +8509,7 @@
       </c>
       <c r="G5">
         <f>SQRT(G3^2+G4^2)</f>
-        <v>9.2716102121417204E-3</v>
+        <v>1.1021165205228471E-2</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -7978,7 +8542,7 @@
       </c>
       <c r="G6">
         <f>G5/L2</f>
-        <v>1.145555565804624E-3</v>
+        <v>1.3617221662282659E-3</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
@@ -8003,7 +8567,7 @@
         <v>-1.2114369350999965E-2</v>
       </c>
       <c r="E7" s="13">
-        <f t="shared" ref="E7:E10" si="2">D7^2</f>
+        <f t="shared" ref="E7:E11" si="2">D7^2</f>
         <v>1.4675794477244731E-4</v>
       </c>
     </row>
@@ -8068,9 +8632,24 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="25">
+        <v>8.1335197047369494</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="0"/>
+        <v>8.0935490943465993</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="1"/>
+        <v>3.9970610390350103E-2</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="2"/>
+        <v>1.5976496949771635E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>

</xml_diff>